<commit_message>
improved xpath for collector
</commit_message>
<xml_diff>
--- a/ExportedData/ExportedAllTags.xlsx
+++ b/ExportedData/ExportedAllTags.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="590">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1000" uniqueCount="595">
   <si>
     <t>TagId</t>
   </si>
@@ -180,6 +180,9 @@
     <t>2020-11-09</t>
   </si>
   <si>
+    <t>2020-11-10</t>
+  </si>
+  <si>
     <t>/Users/Keshab/Desktop/AllImages/1.jpg</t>
   </si>
   <si>
@@ -406,6 +409,18 @@
   </si>
   <si>
     <t>/Users/Keshab/Desktop/AllImages/97.jpg</t>
+  </si>
+  <si>
+    <t>/Users/Keshab/Desktop/fewImages/1.jpg</t>
+  </si>
+  <si>
+    <t>/Users/Keshab/Desktop/fewImages/2.jpg</t>
+  </si>
+  <si>
+    <t>/Users/Keshab/Desktop/fewImages/3.jpg</t>
+  </si>
+  <si>
+    <t>/Users/Keshab/Desktop/fewImages/4.jpg</t>
   </si>
   <si>
     <t>Collector</t>
@@ -2143,7 +2158,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2177,7 +2192,7 @@
         <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -2191,7 +2206,7 @@
         <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -2208,7 +2223,7 @@
         <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2225,7 +2240,7 @@
         <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2242,7 +2257,7 @@
         <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2259,7 +2274,7 @@
         <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -2276,7 +2291,7 @@
         <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2293,7 +2308,7 @@
         <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2310,7 +2325,7 @@
         <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -2327,7 +2342,7 @@
         <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2344,7 +2359,7 @@
         <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2361,7 +2376,7 @@
         <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2378,7 +2393,7 @@
         <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2392,7 +2407,7 @@
         <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -2409,7 +2424,7 @@
         <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2426,7 +2441,7 @@
         <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -2443,7 +2458,7 @@
         <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2457,7 +2472,7 @@
         <v>53</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -2474,7 +2489,7 @@
         <v>53</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -2491,7 +2506,7 @@
         <v>53</v>
       </c>
       <c r="E21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2505,7 +2520,7 @@
         <v>53</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2522,7 +2537,7 @@
         <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -2536,7 +2551,7 @@
         <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -2553,7 +2568,7 @@
         <v>53</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2567,7 +2582,7 @@
         <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2584,7 +2599,7 @@
         <v>53</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -2598,7 +2613,7 @@
         <v>53</v>
       </c>
       <c r="E28" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -2615,7 +2630,7 @@
         <v>53</v>
       </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -2629,7 +2644,7 @@
         <v>53</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2646,7 +2661,7 @@
         <v>53</v>
       </c>
       <c r="E31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2663,7 +2678,7 @@
         <v>53</v>
       </c>
       <c r="E32" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2680,7 +2695,7 @@
         <v>53</v>
       </c>
       <c r="E33" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2697,7 +2712,7 @@
         <v>53</v>
       </c>
       <c r="E34" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -2711,7 +2726,7 @@
         <v>53</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2728,7 +2743,7 @@
         <v>53</v>
       </c>
       <c r="E36" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -2745,7 +2760,7 @@
         <v>53</v>
       </c>
       <c r="E37" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2762,7 +2777,7 @@
         <v>53</v>
       </c>
       <c r="E38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -2776,7 +2791,7 @@
         <v>53</v>
       </c>
       <c r="E39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -2793,7 +2808,7 @@
         <v>53</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -2810,7 +2825,7 @@
         <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2827,7 +2842,7 @@
         <v>53</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -2844,7 +2859,7 @@
         <v>53</v>
       </c>
       <c r="E43" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -2861,7 +2876,7 @@
         <v>53</v>
       </c>
       <c r="E44" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -2878,7 +2893,7 @@
         <v>53</v>
       </c>
       <c r="E45" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -2895,7 +2910,7 @@
         <v>53</v>
       </c>
       <c r="E46" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -2912,7 +2927,7 @@
         <v>53</v>
       </c>
       <c r="E47" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -2929,7 +2944,7 @@
         <v>53</v>
       </c>
       <c r="E48" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -2946,7 +2961,7 @@
         <v>53</v>
       </c>
       <c r="E49" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -2963,7 +2978,7 @@
         <v>53</v>
       </c>
       <c r="E50" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2980,7 +2995,7 @@
         <v>53</v>
       </c>
       <c r="E51" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2997,7 +3012,7 @@
         <v>53</v>
       </c>
       <c r="E52" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3014,7 +3029,7 @@
         <v>53</v>
       </c>
       <c r="E53" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3031,7 +3046,7 @@
         <v>53</v>
       </c>
       <c r="E54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3045,7 +3060,7 @@
         <v>53</v>
       </c>
       <c r="E55" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -3062,7 +3077,7 @@
         <v>53</v>
       </c>
       <c r="E56" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -3079,7 +3094,7 @@
         <v>53</v>
       </c>
       <c r="E57" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -3096,7 +3111,7 @@
         <v>53</v>
       </c>
       <c r="E58" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -3113,7 +3128,7 @@
         <v>53</v>
       </c>
       <c r="E59" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3130,7 +3145,7 @@
         <v>53</v>
       </c>
       <c r="E60" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -3147,7 +3162,7 @@
         <v>53</v>
       </c>
       <c r="E61" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -3164,7 +3179,7 @@
         <v>53</v>
       </c>
       <c r="E62" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -3181,7 +3196,7 @@
         <v>53</v>
       </c>
       <c r="E63" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -3198,7 +3213,7 @@
         <v>53</v>
       </c>
       <c r="E64" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -3215,7 +3230,7 @@
         <v>53</v>
       </c>
       <c r="E65" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -3232,7 +3247,7 @@
         <v>53</v>
       </c>
       <c r="E66" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3249,7 +3264,7 @@
         <v>53</v>
       </c>
       <c r="E67" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3266,7 +3281,7 @@
         <v>53</v>
       </c>
       <c r="E68" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3283,7 +3298,7 @@
         <v>53</v>
       </c>
       <c r="E69" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3300,7 +3315,7 @@
         <v>53</v>
       </c>
       <c r="E70" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -3317,7 +3332,7 @@
         <v>53</v>
       </c>
       <c r="E71" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3334,7 +3349,7 @@
         <v>53</v>
       </c>
       <c r="E72" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3351,7 +3366,7 @@
         <v>53</v>
       </c>
       <c r="E73" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -3368,7 +3383,7 @@
         <v>53</v>
       </c>
       <c r="E74" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3382,7 +3397,7 @@
         <v>53</v>
       </c>
       <c r="E75" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3399,7 +3414,7 @@
         <v>53</v>
       </c>
       <c r="E76" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3416,7 +3431,75 @@
         <v>53</v>
       </c>
       <c r="E77" t="s">
-        <v>129</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>85</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>54</v>
+      </c>
+      <c r="E78" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>86</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>54</v>
+      </c>
+      <c r="E79" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>87</v>
+      </c>
+      <c r="C80" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" t="s">
+        <v>54</v>
+      </c>
+      <c r="E80" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>88</v>
+      </c>
+      <c r="C81" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" t="s">
+        <v>54</v>
+      </c>
+      <c r="E81" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3426,7 +3509,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3437,25 +3520,25 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3466,22 +3549,22 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="F2" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="G2" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="H2" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -3492,22 +3575,22 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="E3" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="G3" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="H3" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -3518,22 +3601,22 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="F4" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="G4" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="H4" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -3544,22 +3627,22 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="E5" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="F5" t="s">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="G5" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="H5" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -3570,25 +3653,25 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="F6" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="G6" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="H6" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I6" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -3599,25 +3682,25 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E7" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="F7" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="G7" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="H7" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I7" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -3628,22 +3711,22 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="F8" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="G8" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="H8" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -3654,22 +3737,22 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="E9" t="s">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="F9" t="s">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="G9" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="H9" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -3680,22 +3763,22 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="E10" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="F10" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="G10" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="H10" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -3706,22 +3789,22 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="F11" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="G11" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="H11" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -3732,22 +3815,22 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D12" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F12" t="s">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="G12" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="H12" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -3758,25 +3841,25 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F13" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="G13" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="H13" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I13" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -3787,25 +3870,25 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="F14" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="G14" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="H14" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I14" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -3816,25 +3899,25 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D15" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E15" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="F15" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="G15" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="H15" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I15" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3845,22 +3928,22 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D16" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E16" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F16" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="G16" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="I16" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -3871,22 +3954,22 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="F17" t="s">
-        <v>265</v>
+        <v>270</v>
       </c>
       <c r="G17" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="H17" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="18" spans="1:9">
@@ -3897,16 +3980,16 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="E18" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="H18" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -3917,19 +4000,19 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E19" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
       <c r="F19" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="G19" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -3940,19 +4023,19 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D20" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="E20" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="F20" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="G20" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
     </row>
     <row r="21" spans="1:9">
@@ -3963,19 +4046,19 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D21" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="E21" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="F21" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="H21" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -3986,22 +4069,22 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D22" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E22" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F22" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="G22" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="H22" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -4012,22 +4095,22 @@
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D23" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E23" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="F23" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="G23" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="H23" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -4038,22 +4121,22 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="E24" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="F24" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="G24" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="H24" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -4064,22 +4147,22 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="E25" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F25" t="s">
-        <v>270</v>
+        <v>275</v>
       </c>
       <c r="G25" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="H25" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -4090,22 +4173,22 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D26" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E26" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="F26" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="G26" t="s">
-        <v>320</v>
+        <v>325</v>
       </c>
       <c r="H26" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -4116,22 +4199,22 @@
         <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D27" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E27" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="F27" t="s">
-        <v>271</v>
+        <v>276</v>
       </c>
       <c r="G27" t="s">
-        <v>321</v>
+        <v>326</v>
       </c>
       <c r="H27" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -4142,22 +4225,22 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D28" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E28" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="F28" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="G28" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="H28" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -4168,22 +4251,22 @@
         <v>29</v>
       </c>
       <c r="C29" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E29" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="F29" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="G29" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="H29" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -4194,22 +4277,22 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D30" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="E30" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
       <c r="F30" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
       <c r="G30" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="H30" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -4220,22 +4303,22 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D31" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E31" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="F31" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G31" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="H31" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -4246,25 +4329,25 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D32" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="E32" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="F32" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="G32" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="H32" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I32" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -4275,22 +4358,22 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="E33" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F33" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="G33" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="H33" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -4301,22 +4384,22 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D34" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="E34" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="G34" t="s">
-        <v>324</v>
+        <v>329</v>
       </c>
       <c r="H34" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I34" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -4327,19 +4410,19 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D35" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E35" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="F35" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="H35" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -4350,25 +4433,25 @@
         <v>37</v>
       </c>
       <c r="C36" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E36" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="F36" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="G36" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="H36" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I36" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -4379,22 +4462,22 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D37" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E37" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="G37" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="H37" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I37" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -4405,25 +4488,25 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E38" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="F38" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="G38" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="H38" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I38" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -4434,19 +4517,19 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D39" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E39" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="F39" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="H39" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -4457,22 +4540,22 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D40" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="E40" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="F40" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="G40" t="s">
-        <v>326</v>
+        <v>331</v>
       </c>
       <c r="H40" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -4483,25 +4566,25 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="E41" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="F41" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="G41" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="H41" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I41" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -4512,25 +4595,25 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="F42" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="G42" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="H42" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I42" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -4541,19 +4624,19 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="F43" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="G43" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="H43" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -4564,25 +4647,25 @@
         <v>47</v>
       </c>
       <c r="C44" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D44" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E44" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="F44" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="G44" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="H44" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I44" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -4593,25 +4676,25 @@
         <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D45" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="E45" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="F45" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="G45" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H45" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I45" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -4622,22 +4705,22 @@
         <v>49</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D46" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E46" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="G46" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H46" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="I46" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -4648,25 +4731,25 @@
         <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D47" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E47" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
       <c r="F47" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="G47" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
       <c r="H47" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="I47" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -4677,25 +4760,25 @@
         <v>51</v>
       </c>
       <c r="C48" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E48" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="F48" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="G48" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="H48" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I48" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -4706,25 +4789,25 @@
         <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D49" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="E49" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="F49" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="G49" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="H49" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="I49" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -4735,22 +4818,22 @@
         <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D50" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="E50" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F50" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="G50" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="I50" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -4761,22 +4844,22 @@
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="E51" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
       <c r="F51" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="G51" t="s">
-        <v>330</v>
+        <v>335</v>
       </c>
       <c r="I51" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -4787,13 +4870,13 @@
         <v>55</v>
       </c>
       <c r="E52" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="F52" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="G52" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -4804,19 +4887,19 @@
         <v>56</v>
       </c>
       <c r="C53" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D53" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="E53" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="F53" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="H53" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -4827,16 +4910,16 @@
         <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="F54" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="G54" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="I54" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -4847,16 +4930,16 @@
         <v>58</v>
       </c>
       <c r="E55" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="F55" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="G55" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="I55" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -4867,19 +4950,19 @@
         <v>59</v>
       </c>
       <c r="D56" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E56" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F56" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="G56" t="s">
-        <v>334</v>
+        <v>339</v>
       </c>
       <c r="H56" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -4890,16 +4973,16 @@
         <v>60</v>
       </c>
       <c r="D57" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E57" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F57" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="H57" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -4910,10 +4993,10 @@
         <v>61</v>
       </c>
       <c r="E58" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="F58" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -4924,10 +5007,10 @@
         <v>62</v>
       </c>
       <c r="E59" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="H59" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -4938,16 +5021,16 @@
         <v>63</v>
       </c>
       <c r="D60" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="E60" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="F60" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="H60" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -4958,13 +5041,13 @@
         <v>64</v>
       </c>
       <c r="E61" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="G61" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="I61" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -4975,16 +5058,16 @@
         <v>66</v>
       </c>
       <c r="E62" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="F62" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="G62" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="I62" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -4995,19 +5078,19 @@
         <v>67</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D63" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="E63" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="F63" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="H63" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -5018,16 +5101,16 @@
         <v>68</v>
       </c>
       <c r="E64" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="F64" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="G64" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="I64" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -5038,13 +5121,13 @@
         <v>69</v>
       </c>
       <c r="D65" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="E65" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="H65" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -5055,13 +5138,13 @@
         <v>71</v>
       </c>
       <c r="E66" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="F66" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="H66" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -5072,10 +5155,10 @@
         <v>72</v>
       </c>
       <c r="E67" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="H67" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -5086,16 +5169,16 @@
         <v>73</v>
       </c>
       <c r="D68" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="E68" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="F68" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="H68" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -5106,13 +5189,13 @@
         <v>75</v>
       </c>
       <c r="E69" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="F69" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="H69" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -5123,16 +5206,16 @@
         <v>76</v>
       </c>
       <c r="E70" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="F70" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="G70" t="s">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="I70" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="71" spans="1:9">
@@ -5143,22 +5226,22 @@
         <v>77</v>
       </c>
       <c r="C71" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D71" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E71" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="F71" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="G71" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="H71" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="1:9">
@@ -5169,16 +5252,16 @@
         <v>79</v>
       </c>
       <c r="E72" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F72" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="G72" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="I72" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="73" spans="1:9">
@@ -5189,16 +5272,16 @@
         <v>80</v>
       </c>
       <c r="E73" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="G73" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="H73" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="I73" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" spans="1:9">
@@ -5209,13 +5292,13 @@
         <v>81</v>
       </c>
       <c r="E74" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="G74" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="I74" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="75" spans="1:9">
@@ -5226,13 +5309,13 @@
         <v>82</v>
       </c>
       <c r="E75" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="G75" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="I75" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="76" spans="1:9">
@@ -5243,22 +5326,22 @@
         <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="D76" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="E76" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="F76" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="G76" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="H76" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
     </row>
     <row r="77" spans="1:9">
@@ -5269,13 +5352,117 @@
         <v>84</v>
       </c>
       <c r="D77" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E77" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="H77" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>85</v>
+      </c>
+      <c r="C78" t="s">
+        <v>142</v>
+      </c>
+      <c r="D78" t="s">
+        <v>144</v>
+      </c>
+      <c r="E78" t="s">
+        <v>185</v>
+      </c>
+      <c r="F78" t="s">
+        <v>260</v>
+      </c>
+      <c r="G78" t="s">
+        <v>309</v>
+      </c>
+      <c r="H78" t="s">
         <v>349</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>86</v>
+      </c>
+      <c r="C79" t="s">
+        <v>142</v>
+      </c>
+      <c r="D79" t="s">
+        <v>153</v>
+      </c>
+      <c r="E79" t="s">
+        <v>195</v>
+      </c>
+      <c r="F79" t="s">
+        <v>266</v>
+      </c>
+      <c r="G79" t="s">
+        <v>315</v>
+      </c>
+      <c r="H79" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>87</v>
+      </c>
+      <c r="C80" t="s">
+        <v>142</v>
+      </c>
+      <c r="D80" t="s">
+        <v>160</v>
+      </c>
+      <c r="E80" t="s">
+        <v>205</v>
+      </c>
+      <c r="F80" t="s">
+        <v>274</v>
+      </c>
+      <c r="G80" t="s">
+        <v>322</v>
+      </c>
+      <c r="H80" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>88</v>
+      </c>
+      <c r="C81" t="s">
+        <v>142</v>
+      </c>
+      <c r="D81" t="s">
+        <v>167</v>
+      </c>
+      <c r="E81" t="s">
+        <v>215</v>
+      </c>
+      <c r="F81" t="s">
+        <v>274</v>
+      </c>
+      <c r="G81" t="s">
+        <v>322</v>
+      </c>
+      <c r="H81" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5296,22 +5483,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5322,22 +5509,22 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="D2" t="s">
-        <v>417</v>
+        <v>422</v>
       </c>
       <c r="E2" t="s">
-        <v>438</v>
+        <v>443</v>
       </c>
       <c r="F2" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="G2" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="H2" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -5348,22 +5535,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="D3" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="E3" t="s">
-        <v>439</v>
+        <v>444</v>
       </c>
       <c r="F3" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="G3" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="H3" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -5374,22 +5561,22 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="D4" t="s">
-        <v>419</v>
+        <v>424</v>
       </c>
       <c r="E4" t="s">
-        <v>440</v>
+        <v>445</v>
       </c>
       <c r="F4" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="G4" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="H4" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -5400,22 +5587,22 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="D5" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="E5" t="s">
-        <v>441</v>
+        <v>446</v>
       </c>
       <c r="F5" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="G5" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H5" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -5426,22 +5613,22 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="D6" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="E6" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="F6" t="s">
-        <v>491</v>
+        <v>496</v>
       </c>
       <c r="G6" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H6" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -5452,22 +5639,22 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="D7" t="s">
-        <v>422</v>
+        <v>427</v>
       </c>
       <c r="E7" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="F7" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="G7" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="H7" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -5478,22 +5665,22 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="D8" t="s">
-        <v>418</v>
+        <v>423</v>
       </c>
       <c r="E8" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="F8" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="G8" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="H8" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5504,22 +5691,22 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="D9" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="E9" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="F9" t="s">
-        <v>494</v>
+        <v>499</v>
       </c>
       <c r="G9" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="H9" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5530,22 +5717,22 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="D10" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="E10" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="F10" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="G10" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H10" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5556,22 +5743,22 @@
         <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="D11" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="E11" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="F11" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="G11" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H11" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -5582,22 +5769,22 @@
         <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="D12" t="s">
-        <v>425</v>
+        <v>430</v>
       </c>
       <c r="E12" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="F12" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="G12" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="H12" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5608,22 +5795,22 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="D13" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="E13" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="F13" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="G13" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H13" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -5634,22 +5821,22 @@
         <v>16</v>
       </c>
       <c r="C14" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="D14" t="s">
-        <v>426</v>
+        <v>431</v>
       </c>
       <c r="E14" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
       <c r="F14" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="G14" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="H14" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -5660,22 +5847,22 @@
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="D15" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="E15" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="F15" t="s">
-        <v>500</v>
+        <v>505</v>
       </c>
       <c r="G15" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H15" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -5686,22 +5873,22 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="D16" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="E16" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="F16" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="G16" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="H16" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -5712,22 +5899,22 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="D17" t="s">
-        <v>424</v>
+        <v>429</v>
       </c>
       <c r="E17" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
       <c r="F17" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="G17" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H17" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -5738,22 +5925,22 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
       <c r="D18" t="s">
-        <v>428</v>
+        <v>433</v>
       </c>
       <c r="E18" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="F18" t="s">
-        <v>503</v>
+        <v>508</v>
       </c>
       <c r="G18" t="s">
-        <v>543</v>
+        <v>548</v>
       </c>
       <c r="H18" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -5764,22 +5951,22 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="D19" t="s">
-        <v>429</v>
+        <v>434</v>
       </c>
       <c r="E19" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="F19" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="G19" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
       <c r="H19" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -5790,22 +5977,22 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="D20" t="s">
-        <v>423</v>
+        <v>428</v>
       </c>
       <c r="E20" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="F20" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="G20" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="H20" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -5816,22 +6003,22 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="D21" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="E21" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="F21" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="G21" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H21" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -5842,22 +6029,22 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="D22" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="E22" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="F22" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="G22" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="H22" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -5868,22 +6055,22 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="D23" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="E23" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
       <c r="F23" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="G23" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="H23" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -5894,22 +6081,22 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="D24" t="s">
-        <v>421</v>
+        <v>426</v>
       </c>
       <c r="E24" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="F24" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="G24" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H24" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -5920,22 +6107,22 @@
         <v>27</v>
       </c>
       <c r="C25" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="D25" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="E25" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="F25" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="G25" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="H25" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -5946,22 +6133,22 @@
         <v>28</v>
       </c>
       <c r="C26" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="D26" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="E26" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="F26" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="G26" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="H26" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -5972,22 +6159,22 @@
         <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="D27" t="s">
-        <v>427</v>
+        <v>432</v>
       </c>
       <c r="E27" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="F27" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="G27" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H27" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -5998,22 +6185,22 @@
         <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="D28" t="s">
-        <v>420</v>
+        <v>425</v>
       </c>
       <c r="E28" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="F28" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="G28" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="H28" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -6024,19 +6211,19 @@
         <v>31</v>
       </c>
       <c r="C29" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E29" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="F29" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="G29" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="H29" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -6047,22 +6234,22 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="D30" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="E30" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="F30" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="G30" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="H30" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -6073,22 +6260,22 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="D31" t="s">
-        <v>435</v>
+        <v>440</v>
       </c>
       <c r="E31" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="F31" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="G31" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H31" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -6099,19 +6286,19 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E32" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="F32" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="G32" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H32" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -6122,19 +6309,19 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="E33" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="F33" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="G33" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="H33" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -6145,19 +6332,19 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="E34" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="F34" t="s">
-        <v>519</v>
+        <v>524</v>
       </c>
       <c r="G34" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="H34" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -6168,19 +6355,19 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E35" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="F35" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="G35" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="H35" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -6191,19 +6378,19 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E36" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="F36" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="G36" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="H36" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -6214,19 +6401,19 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E37" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="F37" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="G37" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="H37" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -6237,19 +6424,19 @@
         <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E38" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="F38" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="G38" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="H38" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -6260,19 +6447,19 @@
         <v>41</v>
       </c>
       <c r="C39" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="E39" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="F39" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="G39" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H39" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -6283,19 +6470,19 @@
         <v>42</v>
       </c>
       <c r="C40" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E40" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="F40" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="G40" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H40" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -6306,19 +6493,19 @@
         <v>43</v>
       </c>
       <c r="C41" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E41" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="F41" t="s">
-        <v>526</v>
+        <v>531</v>
       </c>
       <c r="G41" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H41" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -6329,19 +6516,19 @@
         <v>44</v>
       </c>
       <c r="C42" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E42" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="F42" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="G42" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H42" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -6352,22 +6539,22 @@
         <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="D43" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="E43" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="F43" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="G43" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H43" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -6378,19 +6565,19 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E44" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="F44" t="s">
-        <v>529</v>
+        <v>534</v>
       </c>
       <c r="G44" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H44" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -6401,19 +6588,19 @@
         <v>47</v>
       </c>
       <c r="C45" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E45" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="F45" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="G45" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="H45" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -6424,22 +6611,22 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="D46" t="s">
-        <v>437</v>
+        <v>442</v>
       </c>
       <c r="E46" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="F46" t="s">
-        <v>531</v>
+        <v>536</v>
       </c>
       <c r="G46" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="H46" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -6450,19 +6637,19 @@
         <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E47" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="F47" t="s">
-        <v>532</v>
+        <v>537</v>
       </c>
       <c r="G47" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H47" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -6473,19 +6660,19 @@
         <v>50</v>
       </c>
       <c r="C48" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E48" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="F48" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="G48" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H48" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -6496,19 +6683,19 @@
         <v>51</v>
       </c>
       <c r="C49" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E49" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="F49" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="G49" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="H49" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -6519,19 +6706,19 @@
         <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="E50" t="s">
-        <v>486</v>
+        <v>491</v>
       </c>
       <c r="F50" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="G50" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="H50" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>